<commit_message>
Se generan reportes de auditoria de 8 am a 8pm
</commit_message>
<xml_diff>
--- a/Proyecto/Campos BD.xlsx
+++ b/Proyecto/Campos BD.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\trendit\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E72348DB-79A1-4265-B30B-F2BE315A2376}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4C2EEBE-EA19-47AE-AA21-6D2450A1383D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9265C945-65BD-4C44-9338-B226AFD77C27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{9265C945-65BD-4C44-9338-B226AFD77C27}"/>
   </bookViews>
   <sheets>
     <sheet name="BD's AU" sheetId="1" r:id="rId1"/>
@@ -1362,9 +1362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6183BCCE-6C21-4DFF-9222-9AB536634A7A}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2208,6 +2209,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2596050-143B-474B-B6B4-5FD66493DF49}">
+  <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2382,9 +2384,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3494EF71-0E32-4D54-9003-7DF80257FABE}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -2927,6 +2930,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D174EE1E-DAC8-4F50-ADCA-0A7ABFAE4279}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3083,6 +3087,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1316F5-F0A1-4FCD-A359-428BAD9CF065}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3261,6 +3266,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CA49FD-E6CF-4BA6-8905-2D423200B35C}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3582,6 +3588,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50133865-59E1-4935-9080-ACC83E8FE744}">
+  <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3723,6 +3730,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6956BD7A-EA9D-4FB2-8353-A0F46CA8E2A7}">
+  <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3985,6 +3993,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698B8C54-7C40-4FE8-B080-610AAB1FC39B}">
+  <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
@@ -4456,6 +4465,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAF0B34-23C3-4ED4-AA0B-44DEC73B05DE}">
+  <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">

</xml_diff>